<commit_message>
Champions tras sorteo oficial
</commit_message>
<xml_diff>
--- a/2026/data/calendario_grupos.xlsx
+++ b/2026/data/calendario_grupos.xlsx
@@ -488,312 +488,312 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ruso VS Lope</t>
+          <t>Armada VS Papu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ruso VS Papu</t>
+          <t>Armada VS Kike</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ruso VS Tony</t>
+          <t>Armada VS Kero</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ruso VS Kero</t>
+          <t>Armada VS Palop</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ruso VS Fale</t>
+          <t>Armada VS Tony</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lope VS Ruso</t>
+          <t>Papu VS Armada</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Papu VS Ruso</t>
+          <t>Kike VS Armada</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tony VS Ruso</t>
+          <t>Kero VS Armada</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Kero VS Ruso</t>
+          <t>Palop VS Armada</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Fale VS Ruso</t>
+          <t>Tony VS Armada</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fale VS Papu</t>
+          <t>Tony VS Kike</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lope VS Tony</t>
+          <t>Papu VS Kero</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Papu VS Kero</t>
+          <t>Kike VS Palop</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tony VS Fale</t>
+          <t>Kero VS Tony</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kero VS Lope</t>
+          <t>Palop VS Papu</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Papu VS Fale</t>
+          <t>Kike VS Tony</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tony VS Lope</t>
+          <t>Kero VS Papu</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Kero VS Papu</t>
+          <t>Palop VS Kike</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Fale VS Tony</t>
+          <t>Tony VS Kero</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Lope VS Kero</t>
+          <t>Papu VS Palop</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kero VS Tony</t>
+          <t>Palop VS Kero</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fale VS Kero</t>
+          <t>Tony VS Palop</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lope VS Fale</t>
+          <t>Papu VS Tony</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Papu VS Lope</t>
+          <t>Kike VS Papu</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Kero VS Kike</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Kero VS Palop</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Palop VS Tony</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Tony VS Papu</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Tony VS Kero</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Kero VS Fale</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Fale VS Lope</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Lope VS Papu</t>
+          <t>Papu VS Kike</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Papu VS Tony</t>
+          <t>Kike VS Kero</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Puche VS Palop</t>
+          <t>Fale VS Coquina</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Puche VS Gonzo</t>
+          <t>Fale VS Gonzo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Puche VS Armada</t>
+          <t>Fale VS Puche</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Puche VS Coquina</t>
+          <t>Fale VS Lope</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Puche VS Kike</t>
+          <t>Fale VS Ruso</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Palop VS Puche</t>
+          <t>Coquina VS Fale</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Gonzo VS Puche</t>
+          <t>Gonzo VS Fale</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Armada VS Puche</t>
+          <t>Puche VS Fale</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Coquina VS Puche</t>
+          <t>Lope VS Fale</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Kike VS Puche</t>
+          <t>Ruso VS Fale</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kike VS Gonzo</t>
+          <t>Ruso VS Gonzo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Palop VS Armada</t>
+          <t>Coquina VS Puche</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gonzo VS Coquina</t>
+          <t>Gonzo VS Lope</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Armada VS Kike</t>
+          <t>Puche VS Ruso</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Coquina VS Palop</t>
+          <t>Lope VS Coquina</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gonzo VS Kike</t>
+          <t>Gonzo VS Ruso</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Armada VS Palop</t>
+          <t>Puche VS Coquina</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Coquina VS Gonzo</t>
+          <t>Lope VS Gonzo</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Kike VS Armada</t>
+          <t>Ruso VS Puche</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Palop VS Coquina</t>
+          <t>Coquina VS Lope</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Coquina VS Armada</t>
+          <t>Lope VS Puche</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kike VS Coquina</t>
+          <t>Ruso VS Lope</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Palop VS Kike</t>
+          <t>Coquina VS Ruso</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gonzo VS Palop</t>
+          <t>Gonzo VS Coquina</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Armada VS Gonzo</t>
+          <t>Puche VS Gonzo</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Armada VS Coquina</t>
+          <t>Puche VS Lope</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Coquina VS Kike</t>
+          <t>Lope VS Ruso</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Kike VS Palop</t>
+          <t>Ruso VS Coquina</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Palop VS Gonzo</t>
+          <t>Coquina VS Gonzo</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Gonzo VS Armada</t>
+          <t>Gonzo VS Puche</t>
         </is>
       </c>
     </row>

</xml_diff>